<commit_message>
Make changes to the QA Tests file
</commit_message>
<xml_diff>
--- a/Documentation, Presentation and QA Tests file/QA Tests.xlsx
+++ b/Documentation, Presentation and QA Tests file/QA Tests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\repos\SprintProject-TeamAIM\Documentation, Presentation and QA Tests file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2683AA0-1E48-4A61-BE15-1731F778168F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33E9871-D24F-4615-8412-F0D23B7FA0E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{299A68C8-F238-4918-BE23-37829C974A19}"/>
   </bookViews>
@@ -102,9 +102,6 @@
     <t>Display end game logo and the number of the guessed easter eggs</t>
   </si>
   <si>
-    <t>Display the word "Congratulations" that changes its colours</t>
-  </si>
-  <si>
     <t>All tests have been made by Miroslav Ivanov on 26.02.2021</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display the word "Congratulations" </t>
   </si>
 </sst>
 </file>
@@ -264,12 +264,18 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -279,22 +285,16 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -620,7 +620,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B14"/>
+      <selection activeCell="E14" sqref="E14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,361 +631,416 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="11"/>
+      <c r="I1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="11"/>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="6" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="6" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4">
         <v>2</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="6" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4">
         <v>3</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-    </row>
-    <row r="2" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4">
+        <v>100</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-    </row>
-    <row r="3" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-    </row>
-    <row r="4" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-    </row>
-    <row r="5" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-    </row>
-    <row r="6" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-    </row>
-    <row r="7" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1">
-        <v>100</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="1" t="s">
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="1" t="s">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="K1:N11"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
@@ -1002,61 +1057,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>